<commit_message>
ready to become new nrdc branch
</commit_message>
<xml_diff>
--- a/Projects/timestep106/HDDCDDdata.xlsx
+++ b/Projects/timestep106/HDDCDDdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Logan\Desktop\REEDRRepositories\REEDR\Projects\timestep106\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{896DDDAC-FDE9-4FCD-BE81-764A3FC0729F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC63E02-7E02-496D-82DE-ECCE6AC3460C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -742,7 +742,7 @@
   <dimension ref="A1:H107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>